<commit_message>
2023-07-03 Monday, 16:35:29 Auto Push
</commit_message>
<xml_diff>
--- a/2023-07-03 Monday.xlsx
+++ b/2023-07-03 Monday.xlsx
@@ -482,10 +482,14 @@
           <t>2023-07-03 15:42:30</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr"/>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>2023-07-03 15:50:05</t>
+        </is>
+      </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>OUT</t>
         </is>
       </c>
     </row>

</xml_diff>